<commit_message>
DDL and docs updated
</commit_message>
<xml_diff>
--- a/docs/Diccionario de Datos.xlsx
+++ b/docs/Diccionario de Datos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jose Martin Rivera\Downloads\Avance 1 - Documentación y Diseño\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1CA7976-8F6B-4B4D-AFAF-CF470891072A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45DD6D03-536B-43C4-9A46-F5189AE0EADA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="527" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="532" uniqueCount="90">
   <si>
     <t>Atributo</t>
   </si>
@@ -744,10 +744,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:F128"/>
+  <dimension ref="B2:F129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="A96" workbookViewId="0">
+      <selection activeCell="F79" sqref="F79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1844,14 +1844,16 @@
         <v>82</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D78" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E78" s="1"/>
+      <c r="E78" s="1" t="s">
+        <v>24</v>
+      </c>
       <c r="F78" s="1" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
     </row>
     <row r="79" spans="2:6" ht="17" x14ac:dyDescent="0.4">
@@ -1859,14 +1861,14 @@
         <v>82</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>38</v>
+        <v>7</v>
       </c>
       <c r="D79" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E79" s="1"/>
       <c r="F79" s="1" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
     </row>
     <row r="80" spans="2:6" ht="17" x14ac:dyDescent="0.4">
@@ -1874,14 +1876,14 @@
         <v>82</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>53</v>
+        <v>38</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="E80" s="1"/>
       <c r="F80" s="1" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
     </row>
     <row r="81" spans="2:6" ht="17" x14ac:dyDescent="0.4">
@@ -1889,14 +1891,14 @@
         <v>82</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="E81" s="1"/>
       <c r="F81" s="1" t="s">
-        <v>56</v>
+        <v>8</v>
       </c>
     </row>
     <row r="82" spans="2:6" ht="17" x14ac:dyDescent="0.4">
@@ -1904,14 +1906,14 @@
         <v>82</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>46</v>
+        <v>27</v>
       </c>
       <c r="E82" s="1"/>
       <c r="F82" s="1" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
     </row>
     <row r="83" spans="2:6" ht="17" x14ac:dyDescent="0.4">
@@ -1919,14 +1921,14 @@
         <v>82</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>13</v>
+        <v>46</v>
       </c>
       <c r="E83" s="1"/>
       <c r="F83" s="1" t="s">
-        <v>8</v>
+        <v>47</v>
       </c>
     </row>
     <row r="84" spans="2:6" ht="17" x14ac:dyDescent="0.4">
@@ -1934,14 +1936,14 @@
         <v>82</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D84" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E84" s="1"/>
       <c r="F84" s="1" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
     </row>
     <row r="85" spans="2:6" ht="17" x14ac:dyDescent="0.4">
@@ -1949,14 +1951,14 @@
         <v>82</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>18</v>
+        <v>59</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="E85" s="1"/>
       <c r="F85" s="1" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
     </row>
     <row r="86" spans="2:6" ht="17" x14ac:dyDescent="0.4">
@@ -1964,14 +1966,14 @@
         <v>82</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D86" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E86" s="1"/>
       <c r="F86" s="1" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
     </row>
     <row r="87" spans="2:6" ht="17" x14ac:dyDescent="0.4">
@@ -1979,14 +1981,14 @@
         <v>82</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="E87" s="1"/>
       <c r="F87" s="1" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
     </row>
     <row r="88" spans="2:6" ht="17" x14ac:dyDescent="0.4">
@@ -1994,24 +1996,32 @@
         <v>82</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D88" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E88" s="1"/>
       <c r="F88" s="1" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="89" spans="2:6" ht="17" x14ac:dyDescent="0.4">
-      <c r="B89" s="6"/>
-      <c r="C89" s="6"/>
-      <c r="D89" s="6"/>
-      <c r="E89" s="6"/>
-      <c r="F89" s="6"/>
-    </row>
-    <row r="90" spans="2:6" ht="17.5" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B89" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D89" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E89" s="1"/>
+      <c r="F89" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="90" spans="2:6" ht="17" x14ac:dyDescent="0.4">
       <c r="B90" s="6"/>
       <c r="C90" s="6"/>
       <c r="D90" s="6"/>
@@ -2019,54 +2029,44 @@
       <c r="F90" s="6"/>
     </row>
     <row r="91" spans="2:6" ht="17.5" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B91" s="7" t="s">
+      <c r="B91" s="6"/>
+      <c r="C91" s="6"/>
+      <c r="D91" s="6"/>
+      <c r="E91" s="6"/>
+      <c r="F91" s="6"/>
+    </row>
+    <row r="92" spans="2:6" ht="17.5" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B92" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="C91" s="4" t="s">
+      <c r="C92" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="D91" s="4" t="s">
+      <c r="D92" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="E91" s="4" t="s">
+      <c r="E92" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="F91" s="5" t="s">
+      <c r="F92" s="5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="92" spans="2:6" ht="17" x14ac:dyDescent="0.4">
-      <c r="B92" s="2" t="s">
+    <row r="93" spans="2:6" ht="17" x14ac:dyDescent="0.4">
+      <c r="B93" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="C92" s="2" t="s">
+      <c r="C93" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="D92" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E92" s="2" t="s">
+      <c r="D93" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E93" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F92" s="2" t="s">
+      <c r="F93" s="2" t="s">
         <v>75</v>
-      </c>
-    </row>
-    <row r="93" spans="2:6" ht="17" x14ac:dyDescent="0.4">
-      <c r="B93" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="C93" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D93" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E93" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F93" s="1" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="94" spans="2:6" ht="17" x14ac:dyDescent="0.4">
@@ -2074,7 +2074,7 @@
         <v>83</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>23</v>
+        <v>4</v>
       </c>
       <c r="D94" s="1" t="s">
         <v>5</v>
@@ -2083,7 +2083,7 @@
         <v>24</v>
       </c>
       <c r="F94" s="1" t="s">
-        <v>51</v>
+        <v>25</v>
       </c>
     </row>
     <row r="95" spans="2:6" ht="17" x14ac:dyDescent="0.4">
@@ -2091,7 +2091,7 @@
         <v>83</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>43</v>
+        <v>23</v>
       </c>
       <c r="D95" s="1" t="s">
         <v>5</v>
@@ -2100,7 +2100,7 @@
         <v>24</v>
       </c>
       <c r="F95" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="96" spans="2:6" ht="17" x14ac:dyDescent="0.4">
@@ -2108,7 +2108,7 @@
         <v>83</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>88</v>
+        <v>43</v>
       </c>
       <c r="D96" s="1" t="s">
         <v>5</v>
@@ -2117,7 +2117,7 @@
         <v>24</v>
       </c>
       <c r="F96" s="1" t="s">
-        <v>89</v>
+        <v>52</v>
       </c>
     </row>
     <row r="97" spans="2:6" ht="17" x14ac:dyDescent="0.4">
@@ -2125,14 +2125,16 @@
         <v>83</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>61</v>
+        <v>88</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E97" s="1"/>
+        <v>5</v>
+      </c>
+      <c r="E97" s="1" t="s">
+        <v>24</v>
+      </c>
       <c r="F97" s="1" t="s">
-        <v>8</v>
+        <v>89</v>
       </c>
     </row>
     <row r="98" spans="2:6" ht="17" x14ac:dyDescent="0.4">
@@ -2140,14 +2142,14 @@
         <v>83</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D98" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E98" s="1"/>
       <c r="F98" s="1" t="s">
-        <v>29</v>
+        <v>8</v>
       </c>
     </row>
     <row r="99" spans="2:6" ht="17" x14ac:dyDescent="0.4">
@@ -2155,14 +2157,14 @@
         <v>83</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>39</v>
+        <v>62</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>5</v>
+        <v>27</v>
       </c>
       <c r="E99" s="1"/>
       <c r="F99" s="1" t="s">
-        <v>87</v>
+        <v>29</v>
       </c>
     </row>
     <row r="100" spans="2:6" ht="17" x14ac:dyDescent="0.4">
@@ -2170,14 +2172,14 @@
         <v>83</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D100" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E100" s="1"/>
       <c r="F100" s="1" t="s">
-        <v>20</v>
+        <v>87</v>
       </c>
     </row>
     <row r="101" spans="2:6" ht="17" x14ac:dyDescent="0.4">
@@ -2185,14 +2187,14 @@
         <v>83</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>63</v>
+        <v>38</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="E101" s="1"/>
       <c r="F101" s="1" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
     </row>
     <row r="102" spans="2:6" ht="17" x14ac:dyDescent="0.4">
@@ -2200,10 +2202,10 @@
         <v>83</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="E102" s="1"/>
       <c r="F102" s="1" t="s">
@@ -2215,14 +2217,14 @@
         <v>83</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="E103" s="1"/>
       <c r="F103" s="1" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
     </row>
     <row r="104" spans="2:6" ht="17" x14ac:dyDescent="0.4">
@@ -2230,7 +2232,7 @@
         <v>83</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D104" s="1" t="s">
         <v>5</v>
@@ -2245,7 +2247,7 @@
         <v>83</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D105" s="1" t="s">
         <v>5</v>
@@ -2260,14 +2262,14 @@
         <v>83</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>12</v>
+        <v>67</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="E106" s="1"/>
       <c r="F106" s="1" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
     </row>
     <row r="107" spans="2:6" ht="17" x14ac:dyDescent="0.4">
@@ -2275,14 +2277,14 @@
         <v>83</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="E107" s="1"/>
       <c r="F107" s="1" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
     </row>
     <row r="108" spans="2:6" ht="17" x14ac:dyDescent="0.4">
@@ -2290,14 +2292,14 @@
         <v>83</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D108" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E108" s="1"/>
       <c r="F108" s="1" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
     </row>
     <row r="109" spans="2:6" ht="17" x14ac:dyDescent="0.4">
@@ -2305,14 +2307,14 @@
         <v>83</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="E109" s="1"/>
       <c r="F109" s="1" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
     </row>
     <row r="110" spans="2:6" ht="17" x14ac:dyDescent="0.4">
@@ -2320,24 +2322,32 @@
         <v>83</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D110" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E110" s="1"/>
       <c r="F110" s="1" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="111" spans="2:6" ht="17" x14ac:dyDescent="0.4">
-      <c r="B111" s="6"/>
-      <c r="C111" s="6"/>
-      <c r="D111" s="6"/>
-      <c r="E111" s="6"/>
-      <c r="F111" s="6"/>
-    </row>
-    <row r="112" spans="2:6" ht="17.5" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B111" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C111" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D111" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E111" s="1"/>
+      <c r="F111" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="112" spans="2:6" ht="17" x14ac:dyDescent="0.4">
       <c r="B112" s="6"/>
       <c r="C112" s="6"/>
       <c r="D112" s="6"/>
@@ -2345,54 +2355,44 @@
       <c r="F112" s="6"/>
     </row>
     <row r="113" spans="2:6" ht="17.5" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B113" s="7" t="s">
+      <c r="B113" s="6"/>
+      <c r="C113" s="6"/>
+      <c r="D113" s="6"/>
+      <c r="E113" s="6"/>
+      <c r="F113" s="6"/>
+    </row>
+    <row r="114" spans="2:6" ht="17.5" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B114" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="C113" s="4" t="s">
+      <c r="C114" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="D113" s="4" t="s">
+      <c r="D114" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="E113" s="4" t="s">
+      <c r="E114" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="F113" s="5" t="s">
+      <c r="F114" s="5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="114" spans="2:6" ht="17" x14ac:dyDescent="0.4">
-      <c r="B114" s="2" t="s">
+    <row r="115" spans="2:6" ht="17" x14ac:dyDescent="0.4">
+      <c r="B115" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="C114" s="2" t="s">
+      <c r="C115" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="D114" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E114" s="2" t="s">
+      <c r="D115" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E115" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F114" s="2" t="s">
+      <c r="F115" s="2" t="s">
         <v>75</v>
-      </c>
-    </row>
-    <row r="115" spans="2:6" ht="17" x14ac:dyDescent="0.4">
-      <c r="B115" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="C115" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D115" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E115" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F115" s="1" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="116" spans="2:6" ht="17" x14ac:dyDescent="0.4">
@@ -2400,7 +2400,7 @@
         <v>84</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>43</v>
+        <v>4</v>
       </c>
       <c r="D116" s="1" t="s">
         <v>5</v>
@@ -2409,7 +2409,7 @@
         <v>24</v>
       </c>
       <c r="F116" s="1" t="s">
-        <v>52</v>
+        <v>25</v>
       </c>
     </row>
     <row r="117" spans="2:6" ht="17" x14ac:dyDescent="0.4">
@@ -2417,14 +2417,16 @@
         <v>84</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>7</v>
+        <v>43</v>
       </c>
       <c r="D117" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E117" s="1"/>
+      <c r="E117" s="1" t="s">
+        <v>24</v>
+      </c>
       <c r="F117" s="1" t="s">
-        <v>8</v>
+        <v>52</v>
       </c>
     </row>
     <row r="118" spans="2:6" ht="17" x14ac:dyDescent="0.4">
@@ -2432,14 +2434,14 @@
         <v>84</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>38</v>
+        <v>7</v>
       </c>
       <c r="D118" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E118" s="1"/>
       <c r="F118" s="1" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
     </row>
     <row r="119" spans="2:6" ht="17" x14ac:dyDescent="0.4">
@@ -2447,14 +2449,14 @@
         <v>84</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>69</v>
+        <v>38</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="E119" s="1"/>
       <c r="F119" s="1" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
     </row>
     <row r="120" spans="2:6" ht="17" x14ac:dyDescent="0.4">
@@ -2462,14 +2464,14 @@
         <v>84</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D120" s="1" t="s">
         <v>16</v>
       </c>
       <c r="E120" s="1"/>
       <c r="F120" s="1" t="s">
-        <v>33</v>
+        <v>8</v>
       </c>
     </row>
     <row r="121" spans="2:6" ht="17" x14ac:dyDescent="0.4">
@@ -2477,14 +2479,14 @@
         <v>84</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
       <c r="D121" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="E121" s="1"/>
       <c r="F121" s="1" t="s">
-        <v>8</v>
+        <v>33</v>
       </c>
     </row>
     <row r="122" spans="2:6" ht="17" x14ac:dyDescent="0.4">
@@ -2492,7 +2494,7 @@
         <v>84</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="D122" s="1" t="s">
         <v>13</v>
@@ -2507,14 +2509,14 @@
         <v>84</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D123" s="1" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="E123" s="1"/>
       <c r="F123" s="1" t="s">
-        <v>73</v>
+        <v>8</v>
       </c>
     </row>
     <row r="124" spans="2:6" ht="17" x14ac:dyDescent="0.4">
@@ -2522,14 +2524,14 @@
         <v>84</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>17</v>
+        <v>72</v>
       </c>
       <c r="D124" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E124" s="1"/>
       <c r="F124" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="125" spans="2:6" ht="17" x14ac:dyDescent="0.4">
@@ -2537,14 +2539,14 @@
         <v>84</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D125" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E125" s="1"/>
       <c r="F125" s="1" t="s">
-        <v>8</v>
+        <v>74</v>
       </c>
     </row>
     <row r="126" spans="2:6" ht="17" x14ac:dyDescent="0.4">
@@ -2552,14 +2554,14 @@
         <v>84</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D126" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E126" s="1"/>
       <c r="F126" s="1" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
     </row>
     <row r="127" spans="2:6" ht="17" x14ac:dyDescent="0.4">
@@ -2567,14 +2569,14 @@
         <v>84</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D127" s="1" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="E127" s="1"/>
       <c r="F127" s="1" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
     </row>
     <row r="128" spans="2:6" ht="17" x14ac:dyDescent="0.4">
@@ -2582,13 +2584,28 @@
         <v>84</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D128" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E128" s="1"/>
       <c r="F128" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="129" spans="2:6" ht="17" x14ac:dyDescent="0.4">
+      <c r="B129" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C129" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D129" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E129" s="1"/>
+      <c r="F129" s="1" t="s">
         <v>20</v>
       </c>
     </row>

</xml_diff>